<commit_message>
Updated EDD files for DBTL 1, 2 - corrected rounding
</commit_message>
<xml_diff>
--- a/data/flaviolin/DBTL1/edd_experiment_description.xlsx
+++ b/data/flaviolin/DBTL1/edd_experiment_description.xlsx
@@ -483,7 +483,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>MOPS: 40.0000, Tricine: 4.0000, H3BO3: 0.0037, Glucose: 20.0000, K2SO4: 0.0295, K2HPO4: 3.9954, FeSO4: 0.0428, NH4Cl: 6.4905, MgCl2: 0.2145, NaCl: 197.9165, (NH4)6Mo7O24: 0.0000, CoCl2: 0.0003, CuSO4: 0.0003, MnSO4: 0.0064, ZnSO4: 0.0009</t>
+          <t>MOPS: 40.000000, Tricine: 4.000000, H3BO3: 0.003744, Glucose: 20.000000, K2SO4: 0.029492, K2HPO4: 3.995413, FeSO4: 0.042847, NH4Cl: 6.490478, MgCl2: 0.214493, NaCl: 197.916509, (NH4)6Mo7O24: 0.000016, CoCl2: 0.000254, CuSO4: 0.000309, MnSO4: 0.006371, ZnSO4: 0.000866</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -517,7 +517,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>MOPS: 40.0000, Tricine: 4.0000, H3BO3: 0.0037, Glucose: 20.0000, K2SO4: 0.0295, K2HPO4: 3.9954, FeSO4: 0.0428, NH4Cl: 6.4905, MgCl2: 0.2145, NaCl: 197.9165, (NH4)6Mo7O24: 0.0000, CoCl2: 0.0003, CuSO4: 0.0003, MnSO4: 0.0064, ZnSO4: 0.0009</t>
+          <t>MOPS: 40.000000, Tricine: 4.000000, H3BO3: 0.003744, Glucose: 20.000000, K2SO4: 0.029492, K2HPO4: 3.995413, FeSO4: 0.042847, NH4Cl: 6.490478, MgCl2: 0.214493, NaCl: 197.916509, (NH4)6Mo7O24: 0.000016, CoCl2: 0.000254, CuSO4: 0.000309, MnSO4: 0.006371, ZnSO4: 0.000866</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -551,7 +551,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>MOPS: 40.0000, Tricine: 4.0000, H3BO3: 0.0037, Glucose: 20.0000, K2SO4: 0.0295, K2HPO4: 3.9954, FeSO4: 0.0428, NH4Cl: 6.4905, MgCl2: 0.2145, NaCl: 197.9165, (NH4)6Mo7O24: 0.0000, CoCl2: 0.0003, CuSO4: 0.0003, MnSO4: 0.0064, ZnSO4: 0.0009</t>
+          <t>MOPS: 40.000000, Tricine: 4.000000, H3BO3: 0.003744, Glucose: 20.000000, K2SO4: 0.029492, K2HPO4: 3.995413, FeSO4: 0.042847, NH4Cl: 6.490478, MgCl2: 0.214493, NaCl: 197.916509, (NH4)6Mo7O24: 0.000016, CoCl2: 0.000254, CuSO4: 0.000309, MnSO4: 0.006371, ZnSO4: 0.000866</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -585,7 +585,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>MOPS: 40.0000, Tricine: 4.0000, H3BO3: 0.0037, Glucose: 20.0000, K2SO4: 0.0295, K2HPO4: 3.9954, FeSO4: 0.0428, NH4Cl: 6.4905, MgCl2: 0.2145, NaCl: 197.9165, (NH4)6Mo7O24: 0.0000, CoCl2: 0.0003, CuSO4: 0.0003, MnSO4: 0.0064, ZnSO4: 0.0009</t>
+          <t>MOPS: 40.000000, Tricine: 4.000000, H3BO3: 0.003744, Glucose: 20.000000, K2SO4: 0.029492, K2HPO4: 3.995413, FeSO4: 0.042847, NH4Cl: 6.490478, MgCl2: 0.214493, NaCl: 197.916509, (NH4)6Mo7O24: 0.000016, CoCl2: 0.000254, CuSO4: 0.000309, MnSO4: 0.006371, ZnSO4: 0.000866</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -619,7 +619,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>MOPS: 40.0000, Tricine: 4.0000, H3BO3: 0.0092, Glucose: 20.0000, K2SO4: 0.3805, K2HPO4: 1.1568, FeSO4: 0.0080, NH4Cl: 11.6182, MgCl2: 5.0303, NaCl: 50.6079, (NH4)6Mo7O24: 0.0002, CoCl2: 0.0002, CuSO4: 0.0000, MnSO4: 0.0004, ZnSO4: 0.0003</t>
+          <t>MOPS: 40.000000, Tricine: 4.000000, H3BO3: 0.009185, Glucose: 20.000000, K2SO4: 0.380499, K2HPO4: 1.156774, FeSO4: 0.007971, NH4Cl: 11.618192, MgCl2: 5.030266, NaCl: 50.607910, (NH4)6Mo7O24: 0.000155, CoCl2: 0.000152, CuSO4: 0.000029, MnSO4: 0.000410, ZnSO4: 0.000277</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -653,7 +653,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>MOPS: 40.0000, Tricine: 4.0000, H3BO3: 0.0092, Glucose: 20.0000, K2SO4: 0.3805, K2HPO4: 1.1568, FeSO4: 0.0080, NH4Cl: 11.6182, MgCl2: 5.0303, NaCl: 50.6079, (NH4)6Mo7O24: 0.0002, CoCl2: 0.0002, CuSO4: 0.0000, MnSO4: 0.0004, ZnSO4: 0.0003</t>
+          <t>MOPS: 40.000000, Tricine: 4.000000, H3BO3: 0.009185, Glucose: 20.000000, K2SO4: 0.380499, K2HPO4: 1.156774, FeSO4: 0.007971, NH4Cl: 11.618192, MgCl2: 5.030266, NaCl: 50.607910, (NH4)6Mo7O24: 0.000155, CoCl2: 0.000152, CuSO4: 0.000029, MnSO4: 0.000410, ZnSO4: 0.000277</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -687,7 +687,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>MOPS: 40.0000, Tricine: 4.0000, H3BO3: 0.0092, Glucose: 20.0000, K2SO4: 0.3805, K2HPO4: 1.1568, FeSO4: 0.0080, NH4Cl: 11.6182, MgCl2: 5.0303, NaCl: 50.6079, (NH4)6Mo7O24: 0.0002, CoCl2: 0.0002, CuSO4: 0.0000, MnSO4: 0.0004, ZnSO4: 0.0003</t>
+          <t>MOPS: 40.000000, Tricine: 4.000000, H3BO3: 0.009185, Glucose: 20.000000, K2SO4: 0.380499, K2HPO4: 1.156774, FeSO4: 0.007971, NH4Cl: 11.618192, MgCl2: 5.030266, NaCl: 50.607910, (NH4)6Mo7O24: 0.000155, CoCl2: 0.000152, CuSO4: 0.000029, MnSO4: 0.000410, ZnSO4: 0.000277</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -721,7 +721,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>MOPS: 40.0000, Tricine: 4.0000, H3BO3: 0.0092, Glucose: 20.0000, K2SO4: 0.3805, K2HPO4: 1.1568, FeSO4: 0.0080, NH4Cl: 11.6182, MgCl2: 5.0303, NaCl: 50.6079, (NH4)6Mo7O24: 0.0002, CoCl2: 0.0002, CuSO4: 0.0000, MnSO4: 0.0004, ZnSO4: 0.0003</t>
+          <t>MOPS: 40.000000, Tricine: 4.000000, H3BO3: 0.009185, Glucose: 20.000000, K2SO4: 0.380499, K2HPO4: 1.156774, FeSO4: 0.007971, NH4Cl: 11.618192, MgCl2: 5.030266, NaCl: 50.607910, (NH4)6Mo7O24: 0.000155, CoCl2: 0.000152, CuSO4: 0.000029, MnSO4: 0.000410, ZnSO4: 0.000277</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -755,7 +755,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>MOPS: 40.0000, Tricine: 4.0000, H3BO3: 0.0344, Glucose: 20.0000, K2SO4: 1.4394, K2HPO4: 6.0208, FeSO4: 0.0651, NH4Cl: 7.7375, MgCl2: 4.1526, NaCl: 33.1377, (NH4)6Mo7O24: 0.0001, CoCl2: 0.0020, CuSO4: 0.0006, MnSO4: 0.0053, ZnSO4: 0.0010</t>
+          <t>MOPS: 40.000000, Tricine: 4.000000, H3BO3: 0.034437, Glucose: 20.000000, K2SO4: 1.439441, K2HPO4: 6.020771, FeSO4: 0.065116, NH4Cl: 7.737483, MgCl2: 4.152594, NaCl: 33.137668, (NH4)6Mo7O24: 0.000104, CoCl2: 0.002010, CuSO4: 0.000573, MnSO4: 0.005294, ZnSO4: 0.000998</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -789,7 +789,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>MOPS: 40.0000, Tricine: 4.0000, H3BO3: 0.0344, Glucose: 20.0000, K2SO4: 1.4394, K2HPO4: 6.0208, FeSO4: 0.0651, NH4Cl: 7.7375, MgCl2: 4.1526, NaCl: 33.1377, (NH4)6Mo7O24: 0.0001, CoCl2: 0.0020, CuSO4: 0.0006, MnSO4: 0.0053, ZnSO4: 0.0010</t>
+          <t>MOPS: 40.000000, Tricine: 4.000000, H3BO3: 0.034437, Glucose: 20.000000, K2SO4: 1.439441, K2HPO4: 6.020771, FeSO4: 0.065116, NH4Cl: 7.737483, MgCl2: 4.152594, NaCl: 33.137668, (NH4)6Mo7O24: 0.000104, CoCl2: 0.002010, CuSO4: 0.000573, MnSO4: 0.005294, ZnSO4: 0.000998</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -823,7 +823,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>MOPS: 40.0000, Tricine: 4.0000, H3BO3: 0.0344, Glucose: 20.0000, K2SO4: 1.4394, K2HPO4: 6.0208, FeSO4: 0.0651, NH4Cl: 7.7375, MgCl2: 4.1526, NaCl: 33.1377, (NH4)6Mo7O24: 0.0001, CoCl2: 0.0020, CuSO4: 0.0006, MnSO4: 0.0053, ZnSO4: 0.0010</t>
+          <t>MOPS: 40.000000, Tricine: 4.000000, H3BO3: 0.034437, Glucose: 20.000000, K2SO4: 1.439441, K2HPO4: 6.020771, FeSO4: 0.065116, NH4Cl: 7.737483, MgCl2: 4.152594, NaCl: 33.137668, (NH4)6Mo7O24: 0.000104, CoCl2: 0.002010, CuSO4: 0.000573, MnSO4: 0.005294, ZnSO4: 0.000998</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -857,7 +857,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>MOPS: 40.0000, Tricine: 4.0000, H3BO3: 0.0344, Glucose: 20.0000, K2SO4: 1.4394, K2HPO4: 6.0208, FeSO4: 0.0651, NH4Cl: 7.7375, MgCl2: 4.1526, NaCl: 33.1377, (NH4)6Mo7O24: 0.0001, CoCl2: 0.0020, CuSO4: 0.0006, MnSO4: 0.0053, ZnSO4: 0.0010</t>
+          <t>MOPS: 40.000000, Tricine: 4.000000, H3BO3: 0.034437, Glucose: 20.000000, K2SO4: 1.439441, K2HPO4: 6.020771, FeSO4: 0.065116, NH4Cl: 7.737483, MgCl2: 4.152594, NaCl: 33.137668, (NH4)6Mo7O24: 0.000104, CoCl2: 0.002010, CuSO4: 0.000573, MnSO4: 0.005294, ZnSO4: 0.000998</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -891,7 +891,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>MOPS: 40.0000, Tricine: 4.0000, H3BO3: 0.0311, Glucose: 20.0000, K2SO4: 0.1957, K2HPO4: 2.3751, FeSO4: 0.0217, NH4Cl: 11.0792, MgCl2: 0.9900, NaCl: 400.1444, (NH4)6Mo7O24: 0.0003, CoCl2: 0.0010, CuSO4: 0.0009, MnSO4: 0.0012, ZnSO4: 0.0006</t>
+          <t>MOPS: 40.000000, Tricine: 4.000000, H3BO3: 0.031080, Glucose: 20.000000, K2SO4: 0.195694, K2HPO4: 2.375088, FeSO4: 0.021687, NH4Cl: 11.079187, MgCl2: 0.989965, NaCl: 400.144448, (NH4)6Mo7O24: 0.000252, CoCl2: 0.000974, CuSO4: 0.000855, MnSO4: 0.001168, ZnSO4: 0.000580</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -925,7 +925,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>MOPS: 40.0000, Tricine: 4.0000, H3BO3: 0.0311, Glucose: 20.0000, K2SO4: 0.1957, K2HPO4: 2.3751, FeSO4: 0.0217, NH4Cl: 11.0792, MgCl2: 0.9900, NaCl: 400.1444, (NH4)6Mo7O24: 0.0003, CoCl2: 0.0010, CuSO4: 0.0009, MnSO4: 0.0012, ZnSO4: 0.0006</t>
+          <t>MOPS: 40.000000, Tricine: 4.000000, H3BO3: 0.031080, Glucose: 20.000000, K2SO4: 0.195694, K2HPO4: 2.375088, FeSO4: 0.021687, NH4Cl: 11.079187, MgCl2: 0.989965, NaCl: 400.144448, (NH4)6Mo7O24: 0.000252, CoCl2: 0.000974, CuSO4: 0.000855, MnSO4: 0.001168, ZnSO4: 0.000580</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -959,7 +959,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>MOPS: 40.0000, Tricine: 4.0000, H3BO3: 0.0311, Glucose: 20.0000, K2SO4: 0.1957, K2HPO4: 2.3751, FeSO4: 0.0217, NH4Cl: 11.0792, MgCl2: 0.9900, NaCl: 400.1444, (NH4)6Mo7O24: 0.0003, CoCl2: 0.0010, CuSO4: 0.0009, MnSO4: 0.0012, ZnSO4: 0.0006</t>
+          <t>MOPS: 40.000000, Tricine: 4.000000, H3BO3: 0.031080, Glucose: 20.000000, K2SO4: 0.195694, K2HPO4: 2.375088, FeSO4: 0.021687, NH4Cl: 11.079187, MgCl2: 0.989965, NaCl: 400.144448, (NH4)6Mo7O24: 0.000252, CoCl2: 0.000974, CuSO4: 0.000855, MnSO4: 0.001168, ZnSO4: 0.000580</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -993,7 +993,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>MOPS: 40.0000, Tricine: 4.0000, H3BO3: 0.0311, Glucose: 20.0000, K2SO4: 0.1957, K2HPO4: 2.3751, FeSO4: 0.0217, NH4Cl: 11.0792, MgCl2: 0.9900, NaCl: 400.1444, (NH4)6Mo7O24: 0.0003, CoCl2: 0.0010, CuSO4: 0.0009, MnSO4: 0.0012, ZnSO4: 0.0006</t>
+          <t>MOPS: 40.000000, Tricine: 4.000000, H3BO3: 0.031080, Glucose: 20.000000, K2SO4: 0.195694, K2HPO4: 2.375088, FeSO4: 0.021687, NH4Cl: 11.079187, MgCl2: 0.989965, NaCl: 400.144448, (NH4)6Mo7O24: 0.000252, CoCl2: 0.000974, CuSO4: 0.000855, MnSO4: 0.001168, ZnSO4: 0.000580</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1027,7 +1027,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>MOPS: 40.0000, Tricine: 4.0000, H3BO3: 0.0249, Glucose: 20.0000, K2SO4: 0.2841, K2HPO4: 1.8713, FeSO4: 0.0098, NH4Cl: 9.3670, MgCl2: 0.1070, NaCl: 22.9350, (NH4)6Mo7O24: 0.0000, CoCl2: 0.0004, CuSO4: 0.0004, MnSO4: 0.0004, ZnSO4: 0.0000</t>
+          <t>MOPS: 40.000000, Tricine: 4.000000, H3BO3: 0.024893, Glucose: 20.000000, K2SO4: 0.284127, K2HPO4: 1.871296, FeSO4: 0.009791, NH4Cl: 9.367041, MgCl2: 0.106963, NaCl: 22.935014, (NH4)6Mo7O24: 0.000005, CoCl2: 0.000441, CuSO4: 0.000360, MnSO4: 0.000396, ZnSO4: 0.000045</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1061,7 +1061,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>MOPS: 40.0000, Tricine: 4.0000, H3BO3: 0.0249, Glucose: 20.0000, K2SO4: 0.2841, K2HPO4: 1.8713, FeSO4: 0.0098, NH4Cl: 9.3670, MgCl2: 0.1070, NaCl: 22.9350, (NH4)6Mo7O24: 0.0000, CoCl2: 0.0004, CuSO4: 0.0004, MnSO4: 0.0004, ZnSO4: 0.0000</t>
+          <t>MOPS: 40.000000, Tricine: 4.000000, H3BO3: 0.024893, Glucose: 20.000000, K2SO4: 0.284127, K2HPO4: 1.871296, FeSO4: 0.009791, NH4Cl: 9.367041, MgCl2: 0.106963, NaCl: 22.935014, (NH4)6Mo7O24: 0.000005, CoCl2: 0.000441, CuSO4: 0.000360, MnSO4: 0.000396, ZnSO4: 0.000045</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1095,7 +1095,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>MOPS: 40.0000, Tricine: 4.0000, H3BO3: 0.0249, Glucose: 20.0000, K2SO4: 0.2841, K2HPO4: 1.8713, FeSO4: 0.0098, NH4Cl: 9.3670, MgCl2: 0.1070, NaCl: 22.9350, (NH4)6Mo7O24: 0.0000, CoCl2: 0.0004, CuSO4: 0.0004, MnSO4: 0.0004, ZnSO4: 0.0000</t>
+          <t>MOPS: 40.000000, Tricine: 4.000000, H3BO3: 0.024893, Glucose: 20.000000, K2SO4: 0.284127, K2HPO4: 1.871296, FeSO4: 0.009791, NH4Cl: 9.367041, MgCl2: 0.106963, NaCl: 22.935014, (NH4)6Mo7O24: 0.000005, CoCl2: 0.000441, CuSO4: 0.000360, MnSO4: 0.000396, ZnSO4: 0.000045</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1129,7 +1129,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>MOPS: 40.0000, Tricine: 4.0000, H3BO3: 0.0249, Glucose: 20.0000, K2SO4: 0.2841, K2HPO4: 1.8713, FeSO4: 0.0098, NH4Cl: 9.3670, MgCl2: 0.1070, NaCl: 22.9350, (NH4)6Mo7O24: 0.0000, CoCl2: 0.0004, CuSO4: 0.0004, MnSO4: 0.0004, ZnSO4: 0.0000</t>
+          <t>MOPS: 40.000000, Tricine: 4.000000, H3BO3: 0.024893, Glucose: 20.000000, K2SO4: 0.284127, K2HPO4: 1.871296, FeSO4: 0.009791, NH4Cl: 9.367041, MgCl2: 0.106963, NaCl: 22.935014, (NH4)6Mo7O24: 0.000005, CoCl2: 0.000441, CuSO4: 0.000360, MnSO4: 0.000396, ZnSO4: 0.000045</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1163,7 +1163,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>MOPS: 40.0000, Tricine: 4.0000, H3BO3: 0.0166, Glucose: 20.0000, K2SO4: 0.2559, K2HPO4: 1.0626, FeSO4: 0.0299, NH4Cl: 12.3360, MgCl2: 2.5378, NaCl: 42.0247, (NH4)6Mo7O24: 0.0000, CoCl2: 0.0002, CuSO4: 0.0000, MnSO4: 0.0071, ZnSO4: 0.0005</t>
+          <t>MOPS: 40.000000, Tricine: 4.000000, H3BO3: 0.016562, Glucose: 20.000000, K2SO4: 0.255908, K2HPO4: 1.062554, FeSO4: 0.029932, NH4Cl: 12.336016, MgCl2: 2.537792, NaCl: 42.024681, (NH4)6Mo7O24: 0.000007, CoCl2: 0.000192, CuSO4: 0.000041, MnSO4: 0.007093, ZnSO4: 0.000486</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1197,7 +1197,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>MOPS: 40.0000, Tricine: 4.0000, H3BO3: 0.0166, Glucose: 20.0000, K2SO4: 0.2559, K2HPO4: 1.0626, FeSO4: 0.0299, NH4Cl: 12.3360, MgCl2: 2.5378, NaCl: 42.0247, (NH4)6Mo7O24: 0.0000, CoCl2: 0.0002, CuSO4: 0.0000, MnSO4: 0.0071, ZnSO4: 0.0005</t>
+          <t>MOPS: 40.000000, Tricine: 4.000000, H3BO3: 0.016562, Glucose: 20.000000, K2SO4: 0.255908, K2HPO4: 1.062554, FeSO4: 0.029932, NH4Cl: 12.336016, MgCl2: 2.537792, NaCl: 42.024681, (NH4)6Mo7O24: 0.000007, CoCl2: 0.000192, CuSO4: 0.000041, MnSO4: 0.007093, ZnSO4: 0.000486</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1231,7 +1231,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>MOPS: 40.0000, Tricine: 4.0000, H3BO3: 0.0166, Glucose: 20.0000, K2SO4: 0.2559, K2HPO4: 1.0626, FeSO4: 0.0299, NH4Cl: 12.3360, MgCl2: 2.5378, NaCl: 42.0247, (NH4)6Mo7O24: 0.0000, CoCl2: 0.0002, CuSO4: 0.0000, MnSO4: 0.0071, ZnSO4: 0.0005</t>
+          <t>MOPS: 40.000000, Tricine: 4.000000, H3BO3: 0.016562, Glucose: 20.000000, K2SO4: 0.255908, K2HPO4: 1.062554, FeSO4: 0.029932, NH4Cl: 12.336016, MgCl2: 2.537792, NaCl: 42.024681, (NH4)6Mo7O24: 0.000007, CoCl2: 0.000192, CuSO4: 0.000041, MnSO4: 0.007093, ZnSO4: 0.000486</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1265,7 +1265,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>MOPS: 40.0000, Tricine: 4.0000, H3BO3: 0.0166, Glucose: 20.0000, K2SO4: 0.2559, K2HPO4: 1.0626, FeSO4: 0.0299, NH4Cl: 12.3360, MgCl2: 2.5378, NaCl: 42.0247, (NH4)6Mo7O24: 0.0000, CoCl2: 0.0002, CuSO4: 0.0000, MnSO4: 0.0071, ZnSO4: 0.0005</t>
+          <t>MOPS: 40.000000, Tricine: 4.000000, H3BO3: 0.016562, Glucose: 20.000000, K2SO4: 0.255908, K2HPO4: 1.062554, FeSO4: 0.029932, NH4Cl: 12.336016, MgCl2: 2.537792, NaCl: 42.024681, (NH4)6Mo7O24: 0.000007, CoCl2: 0.000192, CuSO4: 0.000041, MnSO4: 0.007093, ZnSO4: 0.000486</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1299,7 +1299,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>MOPS: 40.0000, Tricine: 4.0000, H3BO3: 0.0018, Glucose: 20.0000, K2SO4: 1.7747, K2HPO4: 0.3248, FeSO4: 0.0043, NH4Cl: 7.8004, MgCl2: 0.7470, NaCl: 441.4702, (NH4)6Mo7O24: 0.0000, CoCl2: 0.0028, CuSO4: 0.0009, MnSO4: 0.0015, ZnSO4: 0.0004</t>
+          <t>MOPS: 40.000000, Tricine: 4.000000, H3BO3: 0.001816, Glucose: 20.000000, K2SO4: 1.774687, K2HPO4: 0.324830, FeSO4: 0.004349, NH4Cl: 7.800423, MgCl2: 0.746968, NaCl: 441.470194, (NH4)6Mo7O24: 0.000021, CoCl2: 0.002819, CuSO4: 0.000928, MnSO4: 0.001514, ZnSO4: 0.000387</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1333,7 +1333,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>MOPS: 40.0000, Tricine: 4.0000, H3BO3: 0.0018, Glucose: 20.0000, K2SO4: 1.7747, K2HPO4: 0.3248, FeSO4: 0.0043, NH4Cl: 7.8004, MgCl2: 0.7470, NaCl: 441.4702, (NH4)6Mo7O24: 0.0000, CoCl2: 0.0028, CuSO4: 0.0009, MnSO4: 0.0015, ZnSO4: 0.0004</t>
+          <t>MOPS: 40.000000, Tricine: 4.000000, H3BO3: 0.001816, Glucose: 20.000000, K2SO4: 1.774687, K2HPO4: 0.324830, FeSO4: 0.004349, NH4Cl: 7.800423, MgCl2: 0.746968, NaCl: 441.470194, (NH4)6Mo7O24: 0.000021, CoCl2: 0.002819, CuSO4: 0.000928, MnSO4: 0.001514, ZnSO4: 0.000387</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1367,7 +1367,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>MOPS: 40.0000, Tricine: 4.0000, H3BO3: 0.0018, Glucose: 20.0000, K2SO4: 1.7747, K2HPO4: 0.3248, FeSO4: 0.0043, NH4Cl: 7.8004, MgCl2: 0.7470, NaCl: 441.4702, (NH4)6Mo7O24: 0.0000, CoCl2: 0.0028, CuSO4: 0.0009, MnSO4: 0.0015, ZnSO4: 0.0004</t>
+          <t>MOPS: 40.000000, Tricine: 4.000000, H3BO3: 0.001816, Glucose: 20.000000, K2SO4: 1.774687, K2HPO4: 0.324830, FeSO4: 0.004349, NH4Cl: 7.800423, MgCl2: 0.746968, NaCl: 441.470194, (NH4)6Mo7O24: 0.000021, CoCl2: 0.002819, CuSO4: 0.000928, MnSO4: 0.001514, ZnSO4: 0.000387</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1401,7 +1401,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>MOPS: 40.0000, Tricine: 4.0000, H3BO3: 0.0018, Glucose: 20.0000, K2SO4: 1.7747, K2HPO4: 0.3248, FeSO4: 0.0043, NH4Cl: 7.8004, MgCl2: 0.7470, NaCl: 441.4702, (NH4)6Mo7O24: 0.0000, CoCl2: 0.0028, CuSO4: 0.0009, MnSO4: 0.0015, ZnSO4: 0.0004</t>
+          <t>MOPS: 40.000000, Tricine: 4.000000, H3BO3: 0.001816, Glucose: 20.000000, K2SO4: 1.774687, K2HPO4: 0.324830, FeSO4: 0.004349, NH4Cl: 7.800423, MgCl2: 0.746968, NaCl: 441.470194, (NH4)6Mo7O24: 0.000021, CoCl2: 0.002819, CuSO4: 0.000928, MnSO4: 0.001514, ZnSO4: 0.000387</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1435,7 +1435,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>MOPS: 40.0000, Tricine: 4.0000, H3BO3: 0.0028, Glucose: 20.0000, K2SO4: 0.9044, K2HPO4: 0.7953, FeSO4: 0.0176, NH4Cl: 8.5269, MgCl2: 2.1287, NaCl: 38.0059, (NH4)6Mo7O24: 0.0001, CoCl2: 0.0007, CuSO4: 0.0002, MnSO4: 0.0001, ZnSO4: 0.0002</t>
+          <t>MOPS: 40.000000, Tricine: 4.000000, H3BO3: 0.002789, Glucose: 20.000000, K2SO4: 0.904382, K2HPO4: 0.795318, FeSO4: 0.017571, NH4Cl: 8.526913, MgCl2: 2.128669, NaCl: 38.005852, (NH4)6Mo7O24: 0.000059, CoCl2: 0.000670, CuSO4: 0.000165, MnSO4: 0.000125, ZnSO4: 0.000247</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1469,7 +1469,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>MOPS: 40.0000, Tricine: 4.0000, H3BO3: 0.0028, Glucose: 20.0000, K2SO4: 0.9044, K2HPO4: 0.7953, FeSO4: 0.0176, NH4Cl: 8.5269, MgCl2: 2.1287, NaCl: 38.0059, (NH4)6Mo7O24: 0.0001, CoCl2: 0.0007, CuSO4: 0.0002, MnSO4: 0.0001, ZnSO4: 0.0002</t>
+          <t>MOPS: 40.000000, Tricine: 4.000000, H3BO3: 0.002789, Glucose: 20.000000, K2SO4: 0.904382, K2HPO4: 0.795318, FeSO4: 0.017571, NH4Cl: 8.526913, MgCl2: 2.128669, NaCl: 38.005852, (NH4)6Mo7O24: 0.000059, CoCl2: 0.000670, CuSO4: 0.000165, MnSO4: 0.000125, ZnSO4: 0.000247</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1503,7 +1503,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>MOPS: 40.0000, Tricine: 4.0000, H3BO3: 0.0028, Glucose: 20.0000, K2SO4: 0.9044, K2HPO4: 0.7953, FeSO4: 0.0176, NH4Cl: 8.5269, MgCl2: 2.1287, NaCl: 38.0059, (NH4)6Mo7O24: 0.0001, CoCl2: 0.0007, CuSO4: 0.0002, MnSO4: 0.0001, ZnSO4: 0.0002</t>
+          <t>MOPS: 40.000000, Tricine: 4.000000, H3BO3: 0.002789, Glucose: 20.000000, K2SO4: 0.904382, K2HPO4: 0.795318, FeSO4: 0.017571, NH4Cl: 8.526913, MgCl2: 2.128669, NaCl: 38.005852, (NH4)6Mo7O24: 0.000059, CoCl2: 0.000670, CuSO4: 0.000165, MnSO4: 0.000125, ZnSO4: 0.000247</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1537,7 +1537,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>MOPS: 40.0000, Tricine: 4.0000, H3BO3: 0.0028, Glucose: 20.0000, K2SO4: 0.9044, K2HPO4: 0.7953, FeSO4: 0.0176, NH4Cl: 8.5269, MgCl2: 2.1287, NaCl: 38.0059, (NH4)6Mo7O24: 0.0001, CoCl2: 0.0007, CuSO4: 0.0002, MnSO4: 0.0001, ZnSO4: 0.0002</t>
+          <t>MOPS: 40.000000, Tricine: 4.000000, H3BO3: 0.002789, Glucose: 20.000000, K2SO4: 0.904382, K2HPO4: 0.795318, FeSO4: 0.017571, NH4Cl: 8.526913, MgCl2: 2.128669, NaCl: 38.005852, (NH4)6Mo7O24: 0.000059, CoCl2: 0.000670, CuSO4: 0.000165, MnSO4: 0.000125, ZnSO4: 0.000247</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1571,7 +1571,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>MOPS: 40.0000, Tricine: 4.0000, H3BO3: 0.0124, Glucose: 20.0000, K2SO4: 0.1865, K2HPO4: 3.3239, FeSO4: 0.0678, NH4Cl: 8.3314, MgCl2: 4.7066, NaCl: 497.4847, (NH4)6Mo7O24: 0.0002, CoCl2: 0.0001, CuSO4: 0.0000, MnSO4: 0.0008, ZnSO4: 0.0000</t>
+          <t>MOPS: 40.000000, Tricine: 4.000000, H3BO3: 0.012395, Glucose: 20.000000, K2SO4: 0.186466, K2HPO4: 3.323911, FeSO4: 0.067838, NH4Cl: 8.331418, MgCl2: 4.706578, NaCl: 497.484672, (NH4)6Mo7O24: 0.000199, CoCl2: 0.000068, CuSO4: 0.000011, MnSO4: 0.000751, ZnSO4: 0.000018</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1605,7 +1605,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>MOPS: 40.0000, Tricine: 4.0000, H3BO3: 0.0124, Glucose: 20.0000, K2SO4: 0.1865, K2HPO4: 3.3239, FeSO4: 0.0678, NH4Cl: 8.3314, MgCl2: 4.7066, NaCl: 497.4847, (NH4)6Mo7O24: 0.0002, CoCl2: 0.0001, CuSO4: 0.0000, MnSO4: 0.0008, ZnSO4: 0.0000</t>
+          <t>MOPS: 40.000000, Tricine: 4.000000, H3BO3: 0.012395, Glucose: 20.000000, K2SO4: 0.186466, K2HPO4: 3.323911, FeSO4: 0.067838, NH4Cl: 8.331418, MgCl2: 4.706578, NaCl: 497.484672, (NH4)6Mo7O24: 0.000199, CoCl2: 0.000068, CuSO4: 0.000011, MnSO4: 0.000751, ZnSO4: 0.000018</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1639,7 +1639,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>MOPS: 40.0000, Tricine: 4.0000, H3BO3: 0.0124, Glucose: 20.0000, K2SO4: 0.1865, K2HPO4: 3.3239, FeSO4: 0.0678, NH4Cl: 8.3314, MgCl2: 4.7066, NaCl: 497.4847, (NH4)6Mo7O24: 0.0002, CoCl2: 0.0001, CuSO4: 0.0000, MnSO4: 0.0008, ZnSO4: 0.0000</t>
+          <t>MOPS: 40.000000, Tricine: 4.000000, H3BO3: 0.012395, Glucose: 20.000000, K2SO4: 0.186466, K2HPO4: 3.323911, FeSO4: 0.067838, NH4Cl: 8.331418, MgCl2: 4.706578, NaCl: 497.484672, (NH4)6Mo7O24: 0.000199, CoCl2: 0.000068, CuSO4: 0.000011, MnSO4: 0.000751, ZnSO4: 0.000018</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1673,7 +1673,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>MOPS: 40.0000, Tricine: 4.0000, H3BO3: 0.0124, Glucose: 20.0000, K2SO4: 0.1865, K2HPO4: 3.3239, FeSO4: 0.0678, NH4Cl: 8.3314, MgCl2: 4.7066, NaCl: 497.4847, (NH4)6Mo7O24: 0.0002, CoCl2: 0.0001, CuSO4: 0.0000, MnSO4: 0.0008, ZnSO4: 0.0000</t>
+          <t>MOPS: 40.000000, Tricine: 4.000000, H3BO3: 0.012395, Glucose: 20.000000, K2SO4: 0.186466, K2HPO4: 3.323911, FeSO4: 0.067838, NH4Cl: 8.331418, MgCl2: 4.706578, NaCl: 497.484672, (NH4)6Mo7O24: 0.000199, CoCl2: 0.000068, CuSO4: 0.000011, MnSO4: 0.000751, ZnSO4: 0.000018</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1707,7 +1707,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>MOPS: 40.0000, Tricine: 4.0000, H3BO3: 0.0047, Glucose: 20.0000, K2SO4: 0.0649, K2HPO4: 4.5981, FeSO4: 0.0415, NH4Cl: 10.5135, MgCl2: 0.3739, NaCl: 232.3194, (NH4)6Mo7O24: 0.0001, CoCl2: 0.0017, CuSO4: 0.0001, MnSO4: 0.0076, ZnSO4: 0.0000</t>
+          <t>MOPS: 40.000000, Tricine: 4.000000, H3BO3: 0.004742, Glucose: 20.000000, K2SO4: 0.064880, K2HPO4: 4.598113, FeSO4: 0.041488, NH4Cl: 10.513500, MgCl2: 0.373878, NaCl: 232.319445, (NH4)6Mo7O24: 0.000138, CoCl2: 0.001727, CuSO4: 0.000063, MnSO4: 0.007646, ZnSO4: 0.000024</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1741,7 +1741,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>MOPS: 40.0000, Tricine: 4.0000, H3BO3: 0.0047, Glucose: 20.0000, K2SO4: 0.0649, K2HPO4: 4.5981, FeSO4: 0.0415, NH4Cl: 10.5135, MgCl2: 0.3739, NaCl: 232.3194, (NH4)6Mo7O24: 0.0001, CoCl2: 0.0017, CuSO4: 0.0001, MnSO4: 0.0076, ZnSO4: 0.0000</t>
+          <t>MOPS: 40.000000, Tricine: 4.000000, H3BO3: 0.004742, Glucose: 20.000000, K2SO4: 0.064880, K2HPO4: 4.598113, FeSO4: 0.041488, NH4Cl: 10.513500, MgCl2: 0.373878, NaCl: 232.319445, (NH4)6Mo7O24: 0.000138, CoCl2: 0.001727, CuSO4: 0.000063, MnSO4: 0.007646, ZnSO4: 0.000024</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1775,7 +1775,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>MOPS: 40.0000, Tricine: 4.0000, H3BO3: 0.0047, Glucose: 20.0000, K2SO4: 0.0649, K2HPO4: 4.5981, FeSO4: 0.0415, NH4Cl: 10.5135, MgCl2: 0.3739, NaCl: 232.3194, (NH4)6Mo7O24: 0.0001, CoCl2: 0.0017, CuSO4: 0.0001, MnSO4: 0.0076, ZnSO4: 0.0000</t>
+          <t>MOPS: 40.000000, Tricine: 4.000000, H3BO3: 0.004742, Glucose: 20.000000, K2SO4: 0.064880, K2HPO4: 4.598113, FeSO4: 0.041488, NH4Cl: 10.513500, MgCl2: 0.373878, NaCl: 232.319445, (NH4)6Mo7O24: 0.000138, CoCl2: 0.001727, CuSO4: 0.000063, MnSO4: 0.007646, ZnSO4: 0.000024</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1809,7 +1809,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>MOPS: 40.0000, Tricine: 4.0000, H3BO3: 0.0047, Glucose: 20.0000, K2SO4: 0.0649, K2HPO4: 4.5981, FeSO4: 0.0415, NH4Cl: 10.5135, MgCl2: 0.3739, NaCl: 232.3194, (NH4)6Mo7O24: 0.0001, CoCl2: 0.0017, CuSO4: 0.0001, MnSO4: 0.0076, ZnSO4: 0.0000</t>
+          <t>MOPS: 40.000000, Tricine: 4.000000, H3BO3: 0.004742, Glucose: 20.000000, K2SO4: 0.064880, K2HPO4: 4.598113, FeSO4: 0.041488, NH4Cl: 10.513500, MgCl2: 0.373878, NaCl: 232.319445, (NH4)6Mo7O24: 0.000138, CoCl2: 0.001727, CuSO4: 0.000063, MnSO4: 0.007646, ZnSO4: 0.000024</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1843,7 +1843,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>MOPS: 40.0000, Tricine: 4.0000, H3BO3: 0.0035, Glucose: 20.0000, K2SO4: 0.1278, K2HPO4: 5.3308, FeSO4: 0.0942, NH4Cl: 9.1373, MgCl2: 3.8869, NaCl: 16.4759, (NH4)6Mo7O24: 0.0000, CoCl2: 0.0013, CuSO4: 0.0001, MnSO4: 0.0005, ZnSO4: 0.0001</t>
+          <t>MOPS: 40.000000, Tricine: 4.000000, H3BO3: 0.003460, Glucose: 20.000000, K2SO4: 0.127824, K2HPO4: 5.330771, FeSO4: 0.094177, NH4Cl: 9.137315, MgCl2: 3.886869, NaCl: 16.475913, (NH4)6Mo7O24: 0.000026, CoCl2: 0.001310, CuSO4: 0.000081, MnSO4: 0.000512, ZnSO4: 0.000096</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1877,7 +1877,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>MOPS: 40.0000, Tricine: 4.0000, H3BO3: 0.0035, Glucose: 20.0000, K2SO4: 0.1278, K2HPO4: 5.3308, FeSO4: 0.0942, NH4Cl: 9.1373, MgCl2: 3.8869, NaCl: 16.4759, (NH4)6Mo7O24: 0.0000, CoCl2: 0.0013, CuSO4: 0.0001, MnSO4: 0.0005, ZnSO4: 0.0001</t>
+          <t>MOPS: 40.000000, Tricine: 4.000000, H3BO3: 0.003460, Glucose: 20.000000, K2SO4: 0.127824, K2HPO4: 5.330771, FeSO4: 0.094177, NH4Cl: 9.137315, MgCl2: 3.886869, NaCl: 16.475913, (NH4)6Mo7O24: 0.000026, CoCl2: 0.001310, CuSO4: 0.000081, MnSO4: 0.000512, ZnSO4: 0.000096</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1911,7 +1911,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>MOPS: 40.0000, Tricine: 4.0000, H3BO3: 0.0035, Glucose: 20.0000, K2SO4: 0.1278, K2HPO4: 5.3308, FeSO4: 0.0942, NH4Cl: 9.1373, MgCl2: 3.8869, NaCl: 16.4759, (NH4)6Mo7O24: 0.0000, CoCl2: 0.0013, CuSO4: 0.0001, MnSO4: 0.0005, ZnSO4: 0.0001</t>
+          <t>MOPS: 40.000000, Tricine: 4.000000, H3BO3: 0.003460, Glucose: 20.000000, K2SO4: 0.127824, K2HPO4: 5.330771, FeSO4: 0.094177, NH4Cl: 9.137315, MgCl2: 3.886869, NaCl: 16.475913, (NH4)6Mo7O24: 0.000026, CoCl2: 0.001310, CuSO4: 0.000081, MnSO4: 0.000512, ZnSO4: 0.000096</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1945,7 +1945,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>MOPS: 40.0000, Tricine: 4.0000, H3BO3: 0.0035, Glucose: 20.0000, K2SO4: 0.1278, K2HPO4: 5.3308, FeSO4: 0.0942, NH4Cl: 9.1373, MgCl2: 3.8869, NaCl: 16.4759, (NH4)6Mo7O24: 0.0000, CoCl2: 0.0013, CuSO4: 0.0001, MnSO4: 0.0005, ZnSO4: 0.0001</t>
+          <t>MOPS: 40.000000, Tricine: 4.000000, H3BO3: 0.003460, Glucose: 20.000000, K2SO4: 0.127824, K2HPO4: 5.330771, FeSO4: 0.094177, NH4Cl: 9.137315, MgCl2: 3.886869, NaCl: 16.475913, (NH4)6Mo7O24: 0.000026, CoCl2: 0.001310, CuSO4: 0.000081, MnSO4: 0.000512, ZnSO4: 0.000096</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1979,7 +1979,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>MOPS: 40.0000, Tricine: 4.0000, H3BO3: 0.0038, Glucose: 20.0000, K2SO4: 0.3118, K2HPO4: 1.3260, FeSO4: 0.0095, NH4Cl: 9.9277, MgCl2: 0.5684, NaCl: 50.7678, (NH4)6Mo7O24: 0.0000, CoCl2: 0.0003, CuSO4: 0.0001, MnSO4: 0.0007, ZnSO4: 0.0001</t>
+          <t>MOPS: 40.000000, Tricine: 4.000000, H3BO3: 0.003797, Glucose: 20.000000, K2SO4: 0.311780, K2HPO4: 1.325974, FeSO4: 0.009506, NH4Cl: 9.927665, MgCl2: 0.568441, NaCl: 50.767801, (NH4)6Mo7O24: 0.000030, CoCl2: 0.000296, CuSO4: 0.000096, MnSO4: 0.000729, ZnSO4: 0.000102</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -2013,7 +2013,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>MOPS: 40.0000, Tricine: 4.0000, H3BO3: 0.0038, Glucose: 20.0000, K2SO4: 0.3118, K2HPO4: 1.3260, FeSO4: 0.0095, NH4Cl: 9.9277, MgCl2: 0.5684, NaCl: 50.7678, (NH4)6Mo7O24: 0.0000, CoCl2: 0.0003, CuSO4: 0.0001, MnSO4: 0.0007, ZnSO4: 0.0001</t>
+          <t>MOPS: 40.000000, Tricine: 4.000000, H3BO3: 0.003797, Glucose: 20.000000, K2SO4: 0.311780, K2HPO4: 1.325974, FeSO4: 0.009506, NH4Cl: 9.927665, MgCl2: 0.568441, NaCl: 50.767801, (NH4)6Mo7O24: 0.000030, CoCl2: 0.000296, CuSO4: 0.000096, MnSO4: 0.000729, ZnSO4: 0.000102</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -2047,7 +2047,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>MOPS: 40.0000, Tricine: 4.0000, H3BO3: 0.0038, Glucose: 20.0000, K2SO4: 0.3118, K2HPO4: 1.3260, FeSO4: 0.0095, NH4Cl: 9.9277, MgCl2: 0.5684, NaCl: 50.7678, (NH4)6Mo7O24: 0.0000, CoCl2: 0.0003, CuSO4: 0.0001, MnSO4: 0.0007, ZnSO4: 0.0001</t>
+          <t>MOPS: 40.000000, Tricine: 4.000000, H3BO3: 0.003797, Glucose: 20.000000, K2SO4: 0.311780, K2HPO4: 1.325974, FeSO4: 0.009506, NH4Cl: 9.927665, MgCl2: 0.568441, NaCl: 50.767801, (NH4)6Mo7O24: 0.000030, CoCl2: 0.000296, CuSO4: 0.000096, MnSO4: 0.000729, ZnSO4: 0.000102</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -2081,7 +2081,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>MOPS: 40.0000, Tricine: 4.0000, H3BO3: 0.0038, Glucose: 20.0000, K2SO4: 0.3118, K2HPO4: 1.3260, FeSO4: 0.0095, NH4Cl: 9.9277, MgCl2: 0.5684, NaCl: 50.7678, (NH4)6Mo7O24: 0.0000, CoCl2: 0.0003, CuSO4: 0.0001, MnSO4: 0.0007, ZnSO4: 0.0001</t>
+          <t>MOPS: 40.000000, Tricine: 4.000000, H3BO3: 0.003797, Glucose: 20.000000, K2SO4: 0.311780, K2HPO4: 1.325974, FeSO4: 0.009506, NH4Cl: 9.927665, MgCl2: 0.568441, NaCl: 50.767801, (NH4)6Mo7O24: 0.000030, CoCl2: 0.000296, CuSO4: 0.000096, MnSO4: 0.000729, ZnSO4: 0.000102</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">

</xml_diff>